<commit_message>
Tidy up the codes
Classify the codes by moving them to different folders.
</commit_message>
<xml_diff>
--- a/68Bus_SG_IBR.xlsx
+++ b/68Bus_SG_IBR.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\Power-Communication-Isomorphism\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5986DCC3-D997-40AF-AD4D-AB0E7277EA28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56425F7B-FD34-4316-9CDB-E7B266338CF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bus" sheetId="1" r:id="rId1"/>
@@ -3298,7 +3298,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34645F5B-1D7A-4323-9AD6-5FF81941CA24}">
   <dimension ref="A1:J70"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
@@ -3498,7 +3498,7 @@
         <v>0.05</v>
       </c>
       <c r="F10" s="2">
-        <f t="shared" ref="F10:F11" si="5">E10/5</f>
+        <f t="shared" ref="F10" si="5">E10/5</f>
         <v>0.01</v>
       </c>
       <c r="H10">
@@ -3741,7 +3741,7 @@
         <v>0.05</v>
       </c>
       <c r="F22" s="2">
-        <f t="shared" ref="F21:F70" si="11">E22/5</f>
+        <f t="shared" ref="F22:F70" si="11">E22/5</f>
         <v>0.01</v>
       </c>
       <c r="H22">

</xml_diff>